<commit_message>
feat: added serial number to offline tool
- Removed CADID column because they don't use it and it was hidden
- Added serial number column
- Changed layout to include serial number

PS: Important to notice that the upload data will only work correctly after we make all the changes for rename and create serial number column on the database. This works now, but it will add and get the data from the column Model Number that is called serial_number in the database today.

Related work items: #4362, #4371
</commit_message>
<xml_diff>
--- a/OfflineXPlanner/excel_templates/export_assets.xlsx
+++ b/OfflineXPlanner/excel_templates/export_assets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\Trabalho\New System\XPlanner\DEV\OfflineXPlanner\excel_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitProject\xPlannerRepo\OfflineXPlanner\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B37435-D32D-440F-847C-BFDB3D385F08}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E0D4CC-52AC-480A-93EE-3375B0BD853C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{DC0110A3-39B0-4A2F-AC13-CA2C30E7D5ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DC0110A3-39B0-4A2F-AC13-CA2C30E7D5ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -117,14 +117,14 @@
     <t>Mounting Height</t>
   </si>
   <si>
-    <t>CAD ID</t>
+    <t>Serial Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +134,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -161,11 +169,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -184,7 +193,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -480,31 +489,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C802CB-336A-450E-A873-058BA5B3F9E1}">
-  <dimension ref="A1:AE1"/>
+  <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+      <selection activeCell="AE4" sqref="AE4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" customWidth="1"/>
-    <col min="11" max="11" width="11.88671875" customWidth="1"/>
-    <col min="12" max="12" width="16.109375" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
     <col min="14" max="14" width="12" customWidth="1"/>
-    <col min="15" max="15" width="12.44140625" customWidth="1"/>
-    <col min="23" max="23" width="13.88671875" customWidth="1"/>
-    <col min="27" max="27" width="18.44140625" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" customWidth="1"/>
+    <col min="23" max="23" width="13.85546875" customWidth="1"/>
+    <col min="27" max="27" width="18.42578125" customWidth="1"/>
     <col min="29" max="30" width="16" customWidth="1"/>
-    <col min="31" max="31" width="11.6640625" customWidth="1"/>
+    <col min="31" max="31" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -593,11 +602,14 @@
         <v>27</v>
       </c>
       <c r="AD1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="1" t="s">
-        <v>30</v>
-      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>